<commit_message>
foi porra eu sou burro
</commit_message>
<xml_diff>
--- a/entrada_validacao.xlsx
+++ b/entrada_validacao.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tutuc\Dropbox\A - ARTHUR\5o Semestre\TransCal\APS\aps4-mecsol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B48995F-94A8-4362-AEFF-B1C3FBCD20CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2EE97A-0228-4708-B1C2-03D550AF8912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11810" windowHeight="12440" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-13178" windowWidth="23452" windowHeight="12561" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nos" sheetId="1" r:id="rId1"/>
@@ -139,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,13 +166,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -578,26 +571,26 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
+      <c r="A6" s="2">
         <v>0.38400000000000001</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10">
+      <c r="A7" s="2">
         <v>0.432</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="2">
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
+      <c r="A8" s="2">
         <v>0.57599999999999996</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="2">
         <v>0</v>
       </c>
     </row>
@@ -611,7 +604,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
@@ -648,7 +641,7 @@
         <v>193140000000</v>
       </c>
       <c r="D2" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="7">
@@ -667,7 +660,7 @@
         <v>193140000000</v>
       </c>
       <c r="D3" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -684,7 +677,7 @@
         <v>193140000000</v>
       </c>
       <c r="D4" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -698,7 +691,7 @@
         <v>193140000000</v>
       </c>
       <c r="D5" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -712,7 +705,7 @@
         <v>193140000000</v>
       </c>
       <c r="D6" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -726,7 +719,7 @@
         <v>193140000000</v>
       </c>
       <c r="D7" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -740,7 +733,7 @@
         <v>193140000000</v>
       </c>
       <c r="D8" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -754,9 +747,8 @@
         <v>193140000000</v>
       </c>
       <c r="D9" s="3">
-        <v>5.2499999999999997E-4</v>
-      </c>
-      <c r="F9" s="11"/>
+        <v>5.2499999999999997E-6</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -769,7 +761,7 @@
         <v>193140000000</v>
       </c>
       <c r="D10" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -783,7 +775,7 @@
         <v>193140000000</v>
       </c>
       <c r="D11" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -797,7 +789,7 @@
         <v>193140000000</v>
       </c>
       <c r="D12" s="3">
-        <v>5.2499999999999997E-4</v>
+        <v>5.2499999999999997E-6</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -854,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
@@ -915,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2">
-        <v>-1500</v>
+        <v>-1300</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -928,7 +920,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2">
-        <v>-1300</v>
+        <v>-1500</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -941,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>-1500</v>
+        <v>-1300</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -954,7 +946,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2">
-        <v>-1300</v>
+        <v>-1500</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1080,7 +1072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1213,7 +1205,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="12"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>